<commit_message>
Switch to reading sales data from Excel file
Updated loja.py to load data from vendas.xlsx instead of vendas.csv. Adjusted the import statements and commented out the CSV loading line. Also updated vendas.csv and vendas.xlsx with new sales data for FIFA FC 25.
</commit_message>
<xml_diff>
--- a/vendas.xlsx
+++ b/vendas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Professor.SN-303358\Documents\ciencia de dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Professor.SN-303358\Documents\GitHub\ciencia-de-dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B82455-67E9-4E8E-9DED-10C1ECCEFC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97BA4F3-9931-4054-AD71-56ABDF0DD49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{57BA1722-F738-4EDB-846F-B3C663568B3B}"/>
   </bookViews>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FA62D5-9160-4DA3-A0E2-7AD247FC2207}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -551,7 +551,7 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -568,7 +568,7 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -602,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -619,7 +619,7 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -636,7 +636,7 @@
         <v>21</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -653,7 +653,7 @@
         <v>24</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -670,7 +670,7 @@
         <v>19</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>26</v>

</xml_diff>